<commit_message>
push main proj changes to osf dir
</commit_message>
<xml_diff>
--- a/results/tables/Table1.xlsx
+++ b/results/tables/Table1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">ROI</t>
   </si>
@@ -108,6 +108,51 @@
   </si>
   <si>
     <t xml:space="preserve">Lateral Vi / Crus I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOSubcortical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Thalamus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Caudate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Putamen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Pallidum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Hippocampus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Amygdala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Accumbens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Thalamus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Caudate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Putamen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Pallidum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Hippocampus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Amygdala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Accumbens</t>
   </si>
 </sst>
 </file>
@@ -905,6 +950,226 @@
         <v>30</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>